<commit_message>
added @Step annotation, fixed some tests and mistypes
</commit_message>
<xml_diff>
--- a/src/test/resources/DataProviderExcel.xlsx
+++ b/src/test/resources/DataProviderExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zalman\IdeaProjects\petclinic-tests\src\test\java\testsData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanch\IdeaProjects\petclinic-tests\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEED3DC1-76A4-4FAC-B185-83031FFF11D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B850C89A-CA31-49E8-9B53-6C3118C2B957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{70CC0633-4F9E-4E8B-8711-22A68D6F28BD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{70CC0633-4F9E-4E8B-8711-22A68D6F28BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Owner" sheetId="1" r:id="rId1"/>
@@ -255,9 +255,6 @@
     <t>21-55 Antony St.</t>
   </si>
   <si>
-    <t>findUniqOwnerTest</t>
-  </si>
-  <si>
     <t>Thomas</t>
   </si>
   <si>
@@ -565,6 +562,9 @@
   </si>
   <si>
     <t>verifySearchPaginationNumbersTest</t>
+  </si>
+  <si>
+    <t>findUniqueOwnerTest</t>
   </si>
 </sst>
 </file>
@@ -616,21 +616,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -646,9 +642,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -686,7 +682,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -792,7 +788,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -944,21 +940,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C340923-6A96-4169-B9C2-B8FE8B844476}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="37.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="37.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -978,7 +974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -986,7 +982,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -998,7 +994,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1018,7 +1014,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1038,7 +1034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1058,164 +1054,164 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="B10" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="F12" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
         <v>124</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="C13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" t="s">
-        <v>130</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>151</v>
+      <c r="F13" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1228,21 +1224,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E693A0D1-0CCE-48DC-B4A5-2003B8AFC0DF}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="39.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1262,7 +1258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1282,57 +1278,57 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="3" t="s">
         <v>64</v>
       </c>
       <c r="F3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="3" t="s">
         <v>65</v>
       </c>
       <c r="F4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>58</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1342,17 +1338,17 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>59</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1362,232 +1358,232 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>84</v>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>99</v>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>98</v>
       </c>
       <c r="B8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>93</v>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>92</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>100</v>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>99</v>
       </c>
       <c r="B9" t="s">
         <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="D9" t="s">
+        <v>93</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>101</v>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>100</v>
       </c>
       <c r="B10" t="s">
         <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="7" t="s">
         <v>95</v>
       </c>
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
       <c r="E10" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>102</v>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>101</v>
       </c>
       <c r="B11" t="s">
         <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="7" t="s">
         <v>105</v>
       </c>
+      <c r="D11" t="s">
+        <v>104</v>
+      </c>
       <c r="E11" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>103</v>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>102</v>
       </c>
       <c r="B12" t="s">
         <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="7" t="s">
         <v>107</v>
       </c>
+      <c r="D12" t="s">
+        <v>106</v>
+      </c>
       <c r="E12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>104</v>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>103</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="7" t="s">
         <v>109</v>
       </c>
+      <c r="D13" t="s">
+        <v>108</v>
+      </c>
       <c r="E13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" t="s">
         <v>92</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="E15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="B16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="F16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
-      </c>
-      <c r="C17" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
         <v>68</v>
@@ -1598,176 +1594,176 @@
       <c r="E18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="F18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" t="s">
         <v>84</v>
       </c>
-      <c r="B19" t="s">
-        <v>149</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>103</v>
+      <c r="F19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="7" t="s">
         <v>107</v>
       </c>
+      <c r="D20" t="s">
+        <v>106</v>
+      </c>
       <c r="E20" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>100</v>
+        <v>90</v>
+      </c>
+      <c r="F20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
+        <v>93</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" t="s">
         <v>41</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="F22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>149</v>
-      </c>
-      <c r="C23" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="F23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>149</v>
-      </c>
-      <c r="C24" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>104</v>
+      <c r="F24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
-      </c>
-      <c r="D25" s="7" t="s">
         <v>109</v>
       </c>
+      <c r="D25" t="s">
+        <v>108</v>
+      </c>
       <c r="E25" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C26" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C27" t="s">
         <v>68</v>
@@ -1778,99 +1774,99 @@
       <c r="E27" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="F27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" t="s">
         <v>84</v>
       </c>
-      <c r="B28" t="s">
-        <v>149</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="D28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
-        <v>103</v>
+      <c r="F28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="7" t="s">
         <v>107</v>
       </c>
+      <c r="D29" t="s">
+        <v>106</v>
+      </c>
       <c r="E29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>84</v>
+        <v>90</v>
+      </c>
+      <c r="F29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="D30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" t="s">
         <v>168</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" t="s">
-        <v>167</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
@@ -1878,119 +1874,119 @@
       <c r="E32" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" t="s">
+        <v>166</v>
+      </c>
+      <c r="C34" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B33" t="s">
-        <v>167</v>
-      </c>
-      <c r="C33" t="s">
-        <v>171</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F33" s="7" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" t="s">
-        <v>167</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B35" t="s">
-        <v>167</v>
-      </c>
-      <c r="C35" t="s">
-        <v>173</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" t="s">
-        <v>161</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
@@ -1998,68 +1994,68 @@
       <c r="E38" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>102</v>
+      <c r="F38" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>101</v>
       </c>
       <c r="B39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C39" t="s">
+        <v>170</v>
+      </c>
+      <c r="D39" t="s">
+        <v>104</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" t="s">
         <v>171</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" t="s">
-        <v>161</v>
-      </c>
-      <c r="C40" s="7" t="s">
+      <c r="D40" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" t="s">
         <v>172</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B41" t="s">
-        <v>161</v>
-      </c>
-      <c r="C41" t="s">
-        <v>173</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>109</v>
+      <c r="D41" t="s">
+        <v>108</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>175</v>
+        <v>91</v>
+      </c>
+      <c r="F41" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2076,20 +2072,20 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" customWidth="1"/>
     <col min="9" max="9" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2118,12 +2114,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -2147,7 +2143,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -2176,7 +2172,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
@@ -2205,149 +2201,149 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" t="s">
         <v>53</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="H5" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>139</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" t="s">
         <v>141</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="F7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="I6" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="H7" t="s">
         <v>147</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>93</v>
+      <c r="I8" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="F9" t="s">
+        <v>157</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="H9" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="7" t="s">
-        <v>153</v>
+      <c r="I9" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored tests, moved test data preparation methods to BaseTest, added BaseStep with enhanced logs
</commit_message>
<xml_diff>
--- a/src/test/resources/DataProviderExcel.xlsx
+++ b/src/test/resources/DataProviderExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanch\IdeaProjects\petclinic-tests\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B850C89A-CA31-49E8-9B53-6C3118C2B957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B06C3A1-5E58-44A6-8A78-DC5221693B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{70CC0633-4F9E-4E8B-8711-22A68D6F28BD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{70CC0633-4F9E-4E8B-8711-22A68D6F28BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Owner" sheetId="1" r:id="rId1"/>
@@ -477,9 +477,6 @@
     <t>Max</t>
   </si>
   <si>
-    <t>lizrd</t>
-  </si>
-  <si>
     <t>Thompson</t>
   </si>
   <si>
@@ -555,16 +552,19 @@
     <t>3684 Steamboat Ct</t>
   </si>
   <si>
-    <t>verifyClickOnSearchPageNavigatorTest</t>
-  </si>
-  <si>
-    <t>verifyClickOnSearchPageArrowTest</t>
-  </si>
-  <si>
     <t>verifySearchPaginationNumbersTest</t>
   </si>
   <si>
     <t>findUniqueOwnerTest</t>
+  </si>
+  <si>
+    <t>verifyPageNavigationByNumberTest</t>
+  </si>
+  <si>
+    <t>verifyPageNavigationByArrowTest</t>
+  </si>
+  <si>
+    <t>lizard</t>
   </si>
 </sst>
 </file>
@@ -940,7 +940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C340923-6A96-4169-B9C2-B8FE8B844476}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -1071,7 +1071,7 @@
         <v>78</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1091,7 +1091,7 @@
         <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1111,7 +1111,7 @@
         <v>113</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1131,7 +1131,7 @@
         <v>114</v>
       </c>
       <c r="F9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1191,7 +1191,7 @@
         <v>127</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1211,7 +1211,7 @@
         <v>128</v>
       </c>
       <c r="F13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E693A0D1-0CCE-48DC-B4A5-2003B8AFC0DF}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1503,7 +1503,7 @@
         <v>100</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>95</v>
@@ -1515,7 +1515,7 @@
         <v>88</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1523,7 +1523,7 @@
         <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C15" t="s">
         <v>97</v>
@@ -1535,7 +1535,7 @@
         <v>86</v>
       </c>
       <c r="F15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1543,7 +1543,7 @@
         <v>101</v>
       </c>
       <c r="B16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C16" t="s">
         <v>105</v>
@@ -1555,7 +1555,7 @@
         <v>89</v>
       </c>
       <c r="F16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1563,7 +1563,7 @@
         <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C17" t="s">
         <v>70</v>
@@ -1575,7 +1575,7 @@
         <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1583,7 +1583,7 @@
         <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C18" t="s">
         <v>68</v>
@@ -1595,7 +1595,7 @@
         <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1603,7 +1603,7 @@
         <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C19" t="s">
         <v>84</v>
@@ -1615,7 +1615,7 @@
         <v>85</v>
       </c>
       <c r="F19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1623,7 +1623,7 @@
         <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C20" t="s">
         <v>107</v>
@@ -1635,7 +1635,7 @@
         <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1643,7 +1643,7 @@
         <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C21" t="s">
         <v>96</v>
@@ -1655,7 +1655,7 @@
         <v>87</v>
       </c>
       <c r="F21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1663,7 +1663,7 @@
         <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C22" t="s">
         <v>72</v>
@@ -1675,7 +1675,7 @@
         <v>67</v>
       </c>
       <c r="F22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1683,7 +1683,7 @@
         <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C23" t="s">
         <v>71</v>
@@ -1695,7 +1695,7 @@
         <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -1703,7 +1703,7 @@
         <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C24" t="s">
         <v>69</v>
@@ -1715,7 +1715,7 @@
         <v>64</v>
       </c>
       <c r="F24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1723,7 +1723,7 @@
         <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C25" t="s">
         <v>109</v>
@@ -1735,7 +1735,7 @@
         <v>91</v>
       </c>
       <c r="F25" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1743,7 +1743,7 @@
         <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C26" t="s">
         <v>70</v>
@@ -1755,7 +1755,7 @@
         <v>65</v>
       </c>
       <c r="F26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -1763,7 +1763,7 @@
         <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C27" t="s">
         <v>68</v>
@@ -1775,7 +1775,7 @@
         <v>63</v>
       </c>
       <c r="F27" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1783,7 +1783,7 @@
         <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C28" t="s">
         <v>84</v>
@@ -1795,7 +1795,7 @@
         <v>85</v>
       </c>
       <c r="F28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1803,7 +1803,7 @@
         <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C29" t="s">
         <v>107</v>
@@ -1815,7 +1815,7 @@
         <v>90</v>
       </c>
       <c r="F29" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1823,10 +1823,10 @@
         <v>83</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>167</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>77</v>
@@ -1835,7 +1835,7 @@
         <v>85</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1843,10 +1843,10 @@
         <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D31" t="s">
         <v>61</v>
@@ -1855,7 +1855,7 @@
         <v>65</v>
       </c>
       <c r="F31" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1863,10 +1863,10 @@
         <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
@@ -1875,7 +1875,7 @@
         <v>63</v>
       </c>
       <c r="F32" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1883,10 +1883,10 @@
         <v>101</v>
       </c>
       <c r="B33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D33" t="s">
         <v>104</v>
@@ -1895,7 +1895,7 @@
         <v>89</v>
       </c>
       <c r="F33" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1903,10 +1903,10 @@
         <v>98</v>
       </c>
       <c r="B34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D34" t="s">
         <v>92</v>
@@ -1915,7 +1915,7 @@
         <v>86</v>
       </c>
       <c r="F34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1923,10 +1923,10 @@
         <v>103</v>
       </c>
       <c r="B35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D35" t="s">
         <v>108</v>
@@ -1935,7 +1935,7 @@
         <v>91</v>
       </c>
       <c r="F35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -1943,10 +1943,10 @@
         <v>83</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>77</v>
@@ -1955,7 +1955,7 @@
         <v>85</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1963,10 +1963,10 @@
         <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D37" t="s">
         <v>61</v>
@@ -1975,7 +1975,7 @@
         <v>65</v>
       </c>
       <c r="F37" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1983,10 +1983,10 @@
         <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
@@ -1995,7 +1995,7 @@
         <v>63</v>
       </c>
       <c r="F38" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -2003,10 +2003,10 @@
         <v>101</v>
       </c>
       <c r="B39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D39" t="s">
         <v>104</v>
@@ -2015,7 +2015,7 @@
         <v>89</v>
       </c>
       <c r="F39" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -2023,10 +2023,10 @@
         <v>98</v>
       </c>
       <c r="B40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D40" t="s">
         <v>92</v>
@@ -2035,7 +2035,7 @@
         <v>86</v>
       </c>
       <c r="F40" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -2043,10 +2043,10 @@
         <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D41" t="s">
         <v>108</v>
@@ -2055,7 +2055,7 @@
         <v>91</v>
       </c>
       <c r="F41" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2068,8 +2068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{801E78ED-A292-40C3-8AF2-0AFFDEBE85A9}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2256,7 +2256,7 @@
         <v>144</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2282,68 +2282,68 @@
         <v>145</v>
       </c>
       <c r="H7" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="I7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>48</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D9" t="s">
         <v>92</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H9" t="s">
         <v>34</v>
       </c>
       <c r="I9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored search tests, fixed some locators
</commit_message>
<xml_diff>
--- a/src/test/resources/DataProviderExcel.xlsx
+++ b/src/test/resources/DataProviderExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanch\IdeaProjects\petclinic-tests\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B06C3A1-5E58-44A6-8A78-DC5221693B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999F45AF-B7D2-4073-99E5-2082091F9252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{70CC0633-4F9E-4E8B-8711-22A68D6F28BD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{70CC0633-4F9E-4E8B-8711-22A68D6F28BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Owner" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="181">
   <si>
     <t>firstName</t>
   </si>
@@ -565,6 +565,18 @@
   </si>
   <si>
     <t>lizard</t>
+  </si>
+  <si>
+    <t>verifyNoPaginationTest</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>4022 Annandale Rd</t>
+  </si>
+  <si>
+    <t>6085552585</t>
   </si>
 </sst>
 </file>
@@ -1222,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E693A0D1-0CCE-48DC-B4A5-2003B8AFC0DF}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1720,122 +1732,122 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
         <v>147</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F25" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
         <v>147</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>65</v>
       </c>
       <c r="F26" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
         <v>147</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F27" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
         <v>147</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F28" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
         <v>147</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D29" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="F29" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1843,10 +1855,10 @@
         <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="C31" t="s">
-        <v>167</v>
+        <v>70</v>
       </c>
       <c r="D31" t="s">
         <v>61</v>
@@ -1855,7 +1867,7 @@
         <v>65</v>
       </c>
       <c r="F31" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1863,10 +1875,10 @@
         <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="C32" t="s">
-        <v>168</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
@@ -1875,67 +1887,67 @@
         <v>63</v>
       </c>
       <c r="F32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="C33" t="s">
-        <v>169</v>
+        <v>84</v>
       </c>
       <c r="D33" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F33" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>178</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>86</v>
+        <v>180</v>
       </c>
       <c r="F34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B35" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="C35" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="D35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -1943,7 +1955,7 @@
         <v>83</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>166</v>
@@ -1955,7 +1967,7 @@
         <v>85</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1963,7 +1975,7 @@
         <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C37" t="s">
         <v>167</v>
@@ -1975,7 +1987,7 @@
         <v>65</v>
       </c>
       <c r="F37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1983,7 +1995,7 @@
         <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C38" t="s">
         <v>168</v>
@@ -1995,7 +2007,7 @@
         <v>63</v>
       </c>
       <c r="F38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -2003,7 +2015,7 @@
         <v>101</v>
       </c>
       <c r="B39" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C39" t="s">
         <v>169</v>
@@ -2015,7 +2027,7 @@
         <v>89</v>
       </c>
       <c r="F39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -2023,7 +2035,7 @@
         <v>98</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C40" t="s">
         <v>170</v>
@@ -2035,15 +2047,15 @@
         <v>86</v>
       </c>
       <c r="F40" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C41" t="s">
         <v>171</v>
@@ -2055,6 +2067,126 @@
         <v>91</v>
       </c>
       <c r="F41" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" t="s">
+        <v>167</v>
+      </c>
+      <c r="D43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>159</v>
+      </c>
+      <c r="C44" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F44" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" t="s">
+        <v>159</v>
+      </c>
+      <c r="C45" t="s">
+        <v>169</v>
+      </c>
+      <c r="D45" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F45" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" t="s">
+        <v>159</v>
+      </c>
+      <c r="C47" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" t="s">
+        <v>108</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F47" t="s">
         <v>175</v>
       </c>
     </row>
@@ -2068,7 +2200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{801E78ED-A292-40C3-8AF2-0AFFDEBE85A9}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>